<commit_message>
Debugged moving flights; combos lt 3*10**6
</commit_message>
<xml_diff>
--- a/dataSets/PERFORMANCE/algo.xlsx
+++ b/dataSets/PERFORMANCE/algo.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chico\repos\franciscolemos\dfs\dataSets\PERFORMANCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19923807-A2CB-44B1-BC50-163649B595CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94FFCD5-1D80-400B-BFD6-DC6A6AEFB61E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{17FEF333-1069-4381-8225-40FCCD454FF1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{17FEF333-1069-4381-8225-40FCCD454FF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Processor perf." sheetId="1" r:id="rId1"/>
     <sheet name="meshgrid perf." sheetId="2" r:id="rId2"/>
     <sheet name="itertools perf." sheetId="4" r:id="rId3"/>
+    <sheet name="itertools 3m" sheetId="6" r:id="rId4"/>
+    <sheet name="itertools 20m" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'meshgrid perf.'!$A$1:$A$100</definedName>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="14">
   <si>
     <t>AMD Ryzen 7 3750H with Radeon Vega Mobile Gfx [Family 23 Model 24 Stepping 1]</t>
   </si>
@@ -85,8 +87,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.00000E+00"/>
-    <numFmt numFmtId="168" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.000000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -151,11 +153,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -163,6 +165,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2945,6 +2948,1022 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'itertools 3m'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>delta1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'itertools 3m'!$B$2:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>2822400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1058400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>691488</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>483840</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1244160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1881600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>188160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2673000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>362880</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16800</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>403200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>317520</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2187000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>288000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>67200</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>241920</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>282240</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>158400</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1728</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4032</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1020600</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>475200</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>241920</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>42336</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1120</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>34560</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28350</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'itertools 3m'!$D$2:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.61900877952575695</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26483917236328097</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.204976797103882</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.176132917404175</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.417377948760986</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.42698502540588401</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.50878238677979E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.80210995674133301</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.20907473564147899</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.7849884033203099E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.27210378646850603</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.109006643295288</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.67804574966430697</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.11238050460815401</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.09293174743652E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.00207328796387E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.3990154266357401E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.4631433486938504E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.11881828308105501</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.0513725280761705E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.0004043579101599E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.9993057250976602E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.49906682968139698</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.13700819015502899</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.8011293411254897E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.00018978118896E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.0010890960693394E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.0352554321289097E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8DB0-4C39-9B45-913240BC0321}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1159425455"/>
+        <c:axId val="1355635695"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1159425455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1355635695"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1355635695"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1159425455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'itertools 20m'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>delta1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'itertools 20m'!$B$2:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>225792</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2540160</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2483712</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2751840</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>302400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7244160</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3326400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>677376</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>982800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4324320</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2280960</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3638250</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17385984</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>422400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1693440</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2027520</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>458640</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4515840</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>53900</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>898560</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>77760</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10800</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>441000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>94080</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>405000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2694384</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>23040</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>37800</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>112000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>655360</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>217728</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5670</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5840640</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>864000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9313920</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3150</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2794176</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>161700</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1512000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'itertools 20m'!$D$2:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>5.4879188537597698E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.63881087303161599</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79191517829894997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.665213823318481</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.6833505630493199E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.74092364311218</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.49699854850769</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.103009700775146</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.27773475646972701</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.24087858200073</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.57698225975036599</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95375895500183105</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.5250208377838099</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.167247533798218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.37330651283264199</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.42668604850768999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.4004878997802707E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.3689646720886199</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0995388031005899E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.17335414886474601</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.5002489089965799E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.0010471343994102E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.0993413925170898E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.5115251541137699E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.113021612167358</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.74019479751586903</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.2998819351196299E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.6866683959960899E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.82537841796875E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.26865696907043501</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7.4234724044799805E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.9989013671875E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.1958599090576201</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.26998853683471702</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.1751437187194802</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.0004043579101599E-3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.77495455741882302</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.0599098205566399E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.589086294174194</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-48B6-4262-9F0E-0A196DDA5751}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1407242111"/>
+        <c:axId val="1041636703"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1407242111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1041636703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1041636703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1407242111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3065,6 +4084,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4098,6 +5197,1038 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4723,6 +6854,88 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{247D6EFD-D444-4820-8DD6-94F37F89089D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A95C368-9855-4369-8E59-C4BF6A5F5DB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6491,8 +8704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B215158-6636-4715-A17F-B47B14707DAE}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="R38" sqref="R38"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8495,4 +10708,1078 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0AED03-D54C-490A-961A-D63D76C5FD4C}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>2822400</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.61900877952575695</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>1058400</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.26483917236328097</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>691488</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0.204976797103882</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>483840</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.176132917404175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1244160</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.417377948760986</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>112</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1881600</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0.42698502540588401</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>188160</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>3.50878238677979E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2673000</v>
+      </c>
+      <c r="C10">
+        <v>1.2302398681640601E-4</v>
+      </c>
+      <c r="D10">
+        <v>0.80210995674133301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>362880</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.20907473564147899</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>16800</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>5.7849884033203099E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>403200</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0.27210378646850603</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>317520</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.109006643295288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>2187000</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0.67804574966430697</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>288000</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0.11238050460815401</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>21000</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>4.09293174743652E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>6000</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1.00207328796387E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>67200</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>2.3990154266357401E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>241920</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>9.4631433486938504E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>282240</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0.11881828308105501</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>158400</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>7.0513725280761705E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>1728</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1.0004043579101599E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>4032</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>2.9993057250976602E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>1020600</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0.49906682968139698</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>475200</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0.13700819015502899</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>241920</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>5.8011293411254897E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>42336</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>1.00018978118896E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>1120</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>34560</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>8.0010890960693394E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>8</v>
+      </c>
+      <c r="B31">
+        <v>28350</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>7.0352554321289097E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1">
+        <f>SUM(B2:B31)</f>
+        <v>17245166</v>
+      </c>
+      <c r="C32" s="1">
+        <f t="shared" ref="C32:D32" si="0">SUM(C2:C31)</f>
+        <v>1.2302398681640601E-4</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3690876960754403</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E68A9D2-07F2-4D70-A0E9-32668132B1C8}">
+  <dimension ref="A1:D42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:D42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>225792</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5.4879188537597698E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2540160</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.63881087303161599</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2483712</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.79191517829894997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2751840</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.665213823318481</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>302400</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5.6833505630493199E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>7244160</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2.74092364311218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3326400</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.49699854850769</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>677376</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.103009700775146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>982800</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.27773475646972701</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4324320</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.24087858200073</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2280960</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.57698225975036599</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3638250</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.95375895500183105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1">
+        <v>17385984</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>4.5250208377838099</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1">
+        <v>422400</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.167247533798218</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1693440</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.37330651283264199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2027520</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.42668604850768999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1">
+        <v>458640</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>8.4004878997802707E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1">
+        <v>4515840</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.3689646720886199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1">
+        <v>53900</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1.0995388031005899E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1">
+        <v>898560</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.17335414886474601</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1">
+        <v>77760</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.5002489089965799E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1">
+        <v>10800</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2.0010471343994102E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24" s="1">
+        <v>441000</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <v>8.0993413925170898E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25" s="1">
+        <v>94080</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2.5115251541137699E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1">
+        <v>168</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27" s="1">
+        <v>405000</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.113021612167358</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>8</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2694384</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.74019479751586903</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29" s="1">
+        <v>23040</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1.2998819351196299E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1">
+        <v>37800</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1.6866683959960899E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>7</v>
+      </c>
+      <c r="B31" s="1">
+        <v>112000</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>3.82537841796875E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32" s="1">
+        <v>655360</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.26865696907043501</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>8</v>
+      </c>
+      <c r="B33" s="1">
+        <v>217728</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>7.4234724044799805E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1">
+        <v>5670</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1.9989013671875E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>8</v>
+      </c>
+      <c r="B35" s="1">
+        <v>5840640</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1.1958599090576201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>8</v>
+      </c>
+      <c r="B36" s="1">
+        <v>864000</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.26998853683471702</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>9</v>
+      </c>
+      <c r="B37" s="1">
+        <v>9313920</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <v>3.1751437187194802</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>6</v>
+      </c>
+      <c r="B38" s="1">
+        <v>3150</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1.0004043579101599E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39" s="1">
+        <v>2794176</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.77495455741882302</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>7</v>
+      </c>
+      <c r="B40" s="1">
+        <v>161700</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1">
+        <v>5.0599098205566399E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>8</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1512000</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.589086294174194</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="1">
+        <f>SUM(B2:B41)</f>
+        <v>83498830</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" ref="C42:D42" si="0">SUM(C2:C41)</f>
+        <v>0</v>
+      </c>
+      <c r="D42" s="7">
+        <f t="shared" si="0"/>
+        <v>24.173490047454823</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>